<commit_message>
Created new caesar cypher I quickly created a new caesar cypher script to help test the new decryption scheme.
</commit_message>
<xml_diff>
--- a/Dictionary Tools/revised script data.xlsx
+++ b/Dictionary Tools/revised script data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Total Time Elapsed</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>6:55pm eta 3.3243 hrs</t>
+  </si>
+  <si>
+    <t>8:01PM</t>
+  </si>
+  <si>
+    <t>8:59PM</t>
   </si>
 </sst>
 </file>
@@ -205,10 +211,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$20</c:f>
+              <c:f>Sheet1!$E$3:$E$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>233</c:v>
                 </c:pt>
@@ -262,6 +268,90 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>285</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>237</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>308</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>441</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>306</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>244</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>329</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>424</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>534</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>631</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>239</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>322</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>389</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>486</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>639</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>757</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>449</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>389</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>202</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>281</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>169</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -302,10 +392,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$3:$G$20</c:f>
+              <c:f>Sheet1!$G$3:$G$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>2.9886909999999998</c:v>
                 </c:pt>
@@ -359,6 +449,90 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>2.6772782592592592</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.5137028421052627</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.3723430833333334</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.2229844444444442</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.1162199545454543</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.0337463526570052</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.9866937870370369</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.900339626666667</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.7880706367521368</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.6737527119341566</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.5804067500000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.5036235555555557</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.4409762222222222</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.3907173548387095</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.3471082465277777</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.248739232323232</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.1499906078431374</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.0634754666666666</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.98257592283950645</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.907619810810811</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.83976746783625711</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.77316474358974319</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.68402703333333315</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.58566217344173432</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.49248457407407392</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.39230060465116284</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.29565611111111101</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.20187482222222267</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.1079810869565222</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1166,16 +1340,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>215153</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:rowOff>150438</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>522194</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>36138</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1460,10 +1634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1809,7 +1983,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <f>A16+1</f>
         <v>15</v>
@@ -1818,11 +1992,11 @@
         <v>5260</v>
       </c>
       <c r="C17">
-        <f t="shared" ref="C17:C20" si="0">C16+5000</f>
+        <f t="shared" ref="C17:C48" si="0">C16+5000</f>
         <v>75000</v>
       </c>
       <c r="E17">
-        <f t="shared" ref="E17:E20" si="1">B17-B16</f>
+        <f t="shared" ref="E17:E48" si="1">B17-B16</f>
         <v>210</v>
       </c>
       <c r="F17">
@@ -1830,13 +2004,13 @@
         <v>5000</v>
       </c>
       <c r="G17">
-        <f t="shared" ref="G17:G20" si="2">B17*(235886/C17-1)/3600</f>
+        <f t="shared" ref="G17:G48" si="2">B17*(235886/C17-1)/3600</f>
         <v>3.1342976296296299</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" ref="A18:A20" si="3">A17+1</f>
+        <f t="shared" ref="A18:A48" si="3">A17+1</f>
         <v>16</v>
       </c>
       <c r="B18">
@@ -1859,7 +2033,7 @@
         <v>2.9510085833333335</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="3"/>
         <v>17</v>
@@ -1884,7 +2058,7 @@
         <v>2.7913910000000004</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="3"/>
         <v>18</v>
@@ -1907,6 +2081,712 @@
       <c r="G20">
         <f t="shared" si="2"/>
         <v>2.6772782592592592</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>6102</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>95000</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>156</v>
+      </c>
+      <c r="F21">
+        <f>5000</f>
+        <v>5000</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="2"/>
+        <v>2.5137028421052627</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>6285</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>100000</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>183</v>
+      </c>
+      <c r="F22">
+        <f>5000</f>
+        <v>5000</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="2"/>
+        <v>2.3723430833333334</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>6420</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>105000</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>135</v>
+      </c>
+      <c r="F23">
+        <f>5000</f>
+        <v>5000</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="2"/>
+        <v>2.2229844444444442</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>6657</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>110000</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>237</v>
+      </c>
+      <c r="F24">
+        <f>5000</f>
+        <v>5000</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="2"/>
+        <v>2.1162199545454543</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>6965</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>115000</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>308</v>
+      </c>
+      <c r="F25">
+        <f>5000</f>
+        <v>5000</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="2"/>
+        <v>2.0337463526570052</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>7406</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>120000</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>441</v>
+      </c>
+      <c r="F26">
+        <f>5000</f>
+        <v>5000</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="2"/>
+        <v>1.9866937870370369</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>7712</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>125000</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>306</v>
+      </c>
+      <c r="F27">
+        <f>5000</f>
+        <v>5000</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="2"/>
+        <v>1.900339626666667</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>7903</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>130000</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>191</v>
+      </c>
+      <c r="F28">
+        <f>5000</f>
+        <v>5000</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="2"/>
+        <v>1.7880706367521368</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>8063</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>135000</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="F29">
+        <f>5000</f>
+        <v>5000</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="2"/>
+        <v>1.6737527119341566</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>8307</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>140000</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>244</v>
+      </c>
+      <c r="F30">
+        <f>5000</f>
+        <v>5000</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="2"/>
+        <v>1.5804067500000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>8636</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>145000</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="1"/>
+        <v>329</v>
+      </c>
+      <c r="F31">
+        <f>5000</f>
+        <v>5000</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="2"/>
+        <v>1.5036235555555557</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>9060</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>150000</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="1"/>
+        <v>424</v>
+      </c>
+      <c r="F32">
+        <f>5000</f>
+        <v>5000</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="2"/>
+        <v>1.4409762222222222</v>
+      </c>
+      <c r="H32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>9594</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>155000</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="1"/>
+        <v>534</v>
+      </c>
+      <c r="F33">
+        <f>5000</f>
+        <v>5000</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="2"/>
+        <v>1.3907173548387095</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>10225</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>160000</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="1"/>
+        <v>631</v>
+      </c>
+      <c r="F34">
+        <f>5000</f>
+        <v>5000</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="2"/>
+        <v>1.3471082465277777</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>10464</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>165000</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="1"/>
+        <v>239</v>
+      </c>
+      <c r="F35">
+        <f>5000</f>
+        <v>5000</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="2"/>
+        <v>1.248739232323232</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>10682</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>170000</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="1"/>
+        <v>218</v>
+      </c>
+      <c r="F36">
+        <f>5000</f>
+        <v>5000</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="2"/>
+        <v>1.1499906078431374</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>11004</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>175000</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="1"/>
+        <v>322</v>
+      </c>
+      <c r="F37">
+        <f>5000</f>
+        <v>5000</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="2"/>
+        <v>1.0634754666666666</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>11393</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>180000</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="1"/>
+        <v>389</v>
+      </c>
+      <c r="F38">
+        <f>5000</f>
+        <v>5000</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="2"/>
+        <v>0.98257592283950645</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>11879</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>185000</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="1"/>
+        <v>486</v>
+      </c>
+      <c r="F39">
+        <f>5000</f>
+        <v>5000</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="2"/>
+        <v>0.907619810810811</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>12518</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>190000</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="1"/>
+        <v>639</v>
+      </c>
+      <c r="F40">
+        <f>5000</f>
+        <v>5000</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="2"/>
+        <v>0.83976746783625711</v>
+      </c>
+      <c r="H40" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>13275</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>195000</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="1"/>
+        <v>757</v>
+      </c>
+      <c r="F41">
+        <f>5000</f>
+        <v>5000</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="2"/>
+        <v>0.77316474358974319</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>13724</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>200000</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="1"/>
+        <v>449</v>
+      </c>
+      <c r="F42">
+        <f>5000</f>
+        <v>5000</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="2"/>
+        <v>0.68402703333333315</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>13994</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>205000</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="1"/>
+        <v>270</v>
+      </c>
+      <c r="F43">
+        <f>5000</f>
+        <v>5000</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="2"/>
+        <v>0.58566217344173432</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>14383</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>210000</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="1"/>
+        <v>389</v>
+      </c>
+      <c r="F44">
+        <f>5000</f>
+        <v>5000</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="2"/>
+        <v>0.49248457407407392</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>14538</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>215000</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="1"/>
+        <v>155</v>
+      </c>
+      <c r="F45">
+        <f>5000</f>
+        <v>5000</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="2"/>
+        <v>0.39230060465116284</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>14740</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>220000</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="1"/>
+        <v>202</v>
+      </c>
+      <c r="F46">
+        <f>5000</f>
+        <v>5000</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="2"/>
+        <v>0.29565611111111101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>15021</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>225000</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="1"/>
+        <v>281</v>
+      </c>
+      <c r="F47">
+        <f>5000</f>
+        <v>5000</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="2"/>
+        <v>0.20187482222222267</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>15190</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>230000</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="1"/>
+        <v>169</v>
+      </c>
+      <c r="F48">
+        <f>5000</f>
+        <v>5000</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="2"/>
+        <v>0.1079810869565222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>